<commit_message>
Arreglar "2020 - Present" en teaching-experience
</commit_message>
<xml_diff>
--- a/data/teaching-experience_en.xlsx
+++ b/data/teaching-experience_en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309C1062-1657-4EAE-A837-B56B87E3BAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9E3091-5452-45A5-8B45-7E874DCBA07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,15 +63,9 @@
     <t>Bogotá, Colombia</t>
   </si>
   <si>
-    <t>2015-2019</t>
-  </si>
-  <si>
     <t>\href{https://www.usbbog.edu.co/}{Universidad de San Buenaventura de Bogotá}</t>
   </si>
   <si>
-    <t>2013-2014</t>
-  </si>
-  <si>
     <t>\href{https://www.usbmed.edu.co/}{Universidad de San Buenaventura de Medellín - Sede Ibagué}</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
   </si>
   <si>
     <t>Research Degree Project III (2020-2024)</t>
-  </si>
-  <si>
-    <t>2020-2024</t>
   </si>
   <si>
     <t>Advanced Seminar II (Psychology Msc) (2020)</t>
@@ -152,6 +143,15 @@
   </si>
   <si>
     <t>Neuropsychology Lab  (2009)</t>
+  </si>
+  <si>
+    <t>2020 - Present</t>
+  </si>
+  <si>
+    <t>2015 - 2019</t>
+  </si>
+  <si>
+    <t>2013 - 2014</t>
   </si>
 </sst>
 </file>
@@ -654,48 +654,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -976,19 +976,19 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="85.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="85.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,12 +1005,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -1019,24 +1019,24 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -1045,37 +1045,37 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1083,149 +1083,149 @@
         <v>2015</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1233,18 +1233,18 @@
         <v>2009</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>